<commit_message>
Fix stdev parameter passing error
</commit_message>
<xml_diff>
--- a/cpkdata.xlsx
+++ b/cpkdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fortive-my.sharepoint.com/personal/yongbo_cao_fluke_com/Documents/Github_Repo/FlukeCodeTools/CPKTool/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="40" documentId="13_ncr:1_{80208FE7-629E-47C3-8354-C02D17038AF1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{9E30EC4A-F9B6-472B-AC10-F80B8FE0D8D7}"/>
+  <xr:revisionPtr revIDLastSave="49" documentId="13_ncr:1_{80208FE7-629E-47C3-8354-C02D17038AF1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{9EC0AE41-FFFB-4B79-9A81-89EF9820C611}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,19 +42,19 @@
     <t>ambient</t>
   </si>
   <si>
-    <t>18c</t>
+    <t>18C</t>
   </si>
   <si>
-    <t>28c</t>
+    <t>28C</t>
   </si>
   <si>
-    <t>aftercycle</t>
+    <t>after temp. cycle</t>
   </si>
   <si>
-    <t>storage20</t>
+    <t>storage 60C</t>
   </si>
   <si>
-    <t>storage60</t>
+    <t>storage -40C</t>
   </si>
 </sst>
 </file>
@@ -501,21 +501,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" customWidth="1"/>
-    <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="1" max="1" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.109375" customWidth="1"/>
-    <col min="5" max="5" width="13.5546875" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" customWidth="1"/>
+    <col min="5" max="5" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
@@ -546,22 +546,22 @@
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>950.2</v>
+        <v>972.9</v>
       </c>
       <c r="C2" s="2">
-        <v>949.8</v>
+        <v>977.9</v>
       </c>
       <c r="D2" s="2">
-        <v>947</v>
+        <v>979.6</v>
       </c>
       <c r="E2" s="2">
-        <v>948.7</v>
+        <v>979.9</v>
       </c>
       <c r="F2" s="2">
-        <v>946.9</v>
+        <v>982.2</v>
       </c>
       <c r="G2" s="2">
-        <v>947.7</v>
+        <v>982.9</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.3">
@@ -569,22 +569,22 @@
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>949.2</v>
+        <v>973</v>
       </c>
       <c r="C3" s="1">
-        <v>949.2</v>
+        <v>977.6</v>
       </c>
       <c r="D3" s="1">
-        <v>949.1</v>
+        <v>978.3</v>
       </c>
       <c r="E3" s="1">
-        <v>951.6</v>
+        <v>977.3</v>
       </c>
       <c r="F3" s="1">
-        <v>951.1</v>
+        <v>980</v>
       </c>
       <c r="G3" s="1">
-        <v>950.3</v>
+        <v>977.1</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.3">
@@ -592,22 +592,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>948.3</v>
+        <v>971.6</v>
       </c>
       <c r="C4" s="1">
-        <v>950.3</v>
+        <v>977.6</v>
       </c>
       <c r="D4" s="1">
-        <v>948.4</v>
+        <v>977.5</v>
       </c>
       <c r="E4" s="1">
-        <v>948.8</v>
+        <v>978.5</v>
       </c>
       <c r="F4" s="1">
-        <v>951.4</v>
+        <v>974.5</v>
       </c>
       <c r="G4" s="1">
-        <v>948.8</v>
+        <v>976.7</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.3">
@@ -615,22 +615,22 @@
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>947.5</v>
+        <v>976.4</v>
       </c>
       <c r="C5" s="1">
-        <v>949.6</v>
+        <v>980</v>
       </c>
       <c r="D5" s="1">
-        <v>947.7</v>
+        <v>979.2</v>
       </c>
       <c r="E5" s="1">
-        <v>949.7</v>
+        <v>980.4</v>
       </c>
       <c r="F5" s="1">
-        <v>950.1</v>
+        <v>980.5</v>
       </c>
       <c r="G5" s="1">
-        <v>949.5</v>
+        <v>975.9</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.3">
@@ -638,22 +638,22 @@
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>948.7</v>
+        <v>974.6</v>
       </c>
       <c r="C6" s="1">
-        <v>949.9</v>
+        <v>974.8</v>
       </c>
       <c r="D6" s="1">
-        <v>947.9</v>
+        <v>976.2</v>
       </c>
       <c r="E6" s="1">
-        <v>949.3</v>
+        <v>978.6</v>
       </c>
       <c r="F6" s="1">
-        <v>948.1</v>
+        <v>977.2</v>
       </c>
       <c r="G6" s="1">
-        <v>949</v>
+        <v>978.2</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.3">
@@ -661,22 +661,22 @@
         <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>948.4</v>
+        <v>970.9</v>
       </c>
       <c r="C7" s="1">
-        <v>948.1</v>
+        <v>977.2</v>
       </c>
       <c r="D7" s="1">
-        <v>949.6</v>
+        <v>974.8</v>
       </c>
       <c r="E7" s="1">
-        <v>950.1</v>
+        <v>977.4</v>
       </c>
       <c r="F7" s="1">
-        <v>949</v>
+        <v>974.3</v>
       </c>
       <c r="G7" s="1">
-        <v>950.6</v>
+        <v>974.3</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15" x14ac:dyDescent="0.3">
@@ -684,22 +684,22 @@
         <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>948.7</v>
+        <v>970.9</v>
       </c>
       <c r="C8" s="1">
-        <v>948.9</v>
+        <v>973</v>
       </c>
       <c r="D8" s="1">
-        <v>947.2</v>
+        <v>972.3</v>
       </c>
       <c r="E8" s="1">
-        <v>950.2</v>
+        <v>971.6</v>
       </c>
       <c r="F8" s="1">
-        <v>949</v>
+        <v>971.2</v>
       </c>
       <c r="G8" s="1">
-        <v>950.6</v>
+        <v>970</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15" x14ac:dyDescent="0.3">
@@ -707,22 +707,22 @@
         <v>8</v>
       </c>
       <c r="B9" s="1">
-        <v>948.5</v>
+        <v>974</v>
       </c>
       <c r="C9" s="1">
-        <v>948.5</v>
+        <v>978.1</v>
       </c>
       <c r="D9" s="1">
-        <v>946.6</v>
+        <v>978.6</v>
       </c>
       <c r="E9" s="1">
-        <v>950.1</v>
+        <v>982.1</v>
       </c>
       <c r="F9" s="1">
-        <v>949.7</v>
+        <v>981.3</v>
       </c>
       <c r="G9" s="1">
-        <v>948.4</v>
+        <v>981.1</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15" x14ac:dyDescent="0.3">
@@ -730,22 +730,22 @@
         <v>9</v>
       </c>
       <c r="B10" s="1">
-        <v>948.3</v>
+        <v>971.6</v>
       </c>
       <c r="C10" s="1">
-        <v>951</v>
+        <v>974.2</v>
       </c>
       <c r="D10" s="1">
-        <v>947.5</v>
+        <v>977</v>
       </c>
       <c r="E10" s="1">
-        <v>951.9</v>
+        <v>975.1</v>
       </c>
       <c r="F10" s="1">
-        <v>948.5</v>
+        <v>976.9</v>
       </c>
       <c r="G10" s="1">
-        <v>948.2</v>
+        <v>975.8</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15" x14ac:dyDescent="0.3">
@@ -753,22 +753,22 @@
         <v>10</v>
       </c>
       <c r="B11" s="1">
-        <v>948.2</v>
+        <v>971.3</v>
       </c>
       <c r="C11" s="1">
-        <v>948.5</v>
+        <v>974.3</v>
       </c>
       <c r="D11" s="1">
-        <v>947.2</v>
+        <v>976.6</v>
       </c>
       <c r="E11" s="1">
-        <v>951.3</v>
+        <v>975.9</v>
       </c>
       <c r="F11" s="1">
-        <v>945.8</v>
+        <v>976.8</v>
       </c>
       <c r="G11" s="1">
-        <v>949.3</v>
+        <v>975.3</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.3">
@@ -776,22 +776,22 @@
         <v>11</v>
       </c>
       <c r="B12" s="1">
-        <v>949.4</v>
+        <v>973.1</v>
       </c>
       <c r="C12" s="1">
-        <v>949.6</v>
+        <v>979.1</v>
       </c>
       <c r="D12" s="1">
-        <v>949</v>
+        <v>979</v>
       </c>
       <c r="E12" s="1">
-        <v>950.3</v>
+        <v>980</v>
       </c>
       <c r="F12" s="1">
-        <v>951</v>
+        <v>981.1</v>
       </c>
       <c r="G12" s="1">
-        <v>949</v>
+        <v>979.3</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15" x14ac:dyDescent="0.3">
@@ -799,22 +799,22 @@
         <v>12</v>
       </c>
       <c r="B13" s="1">
-        <v>948.4</v>
+        <v>974.2</v>
       </c>
       <c r="C13" s="1">
-        <v>948.9</v>
+        <v>979</v>
       </c>
       <c r="D13" s="1">
-        <v>945.9</v>
+        <v>975.4</v>
       </c>
       <c r="E13" s="1">
-        <v>950.4</v>
+        <v>979.2</v>
       </c>
       <c r="F13" s="1">
-        <v>951.8</v>
+        <v>980.5</v>
       </c>
       <c r="G13" s="1">
-        <v>950.2</v>
+        <v>977.2</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="15" x14ac:dyDescent="0.3">
@@ -822,22 +822,22 @@
         <v>13</v>
       </c>
       <c r="B14" s="1">
-        <v>947.6</v>
+        <v>972</v>
       </c>
       <c r="C14" s="1">
-        <v>950.7</v>
+        <v>981.8</v>
       </c>
       <c r="D14" s="1">
-        <v>947.9</v>
+        <v>979.7</v>
       </c>
       <c r="E14" s="1">
-        <v>947</v>
+        <v>979</v>
       </c>
       <c r="F14" s="1">
-        <v>948.9</v>
+        <v>983</v>
       </c>
       <c r="G14" s="1">
-        <v>948.7</v>
+        <v>979.9</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="15" x14ac:dyDescent="0.3">
@@ -845,22 +845,22 @@
         <v>14</v>
       </c>
       <c r="B15" s="1">
-        <v>948.4</v>
+        <v>973.4</v>
       </c>
       <c r="C15" s="1">
-        <v>950.5</v>
+        <v>979</v>
       </c>
       <c r="D15" s="1">
-        <v>949.4</v>
+        <v>980.7</v>
       </c>
       <c r="E15" s="1">
-        <v>949</v>
+        <v>980.8</v>
       </c>
       <c r="F15" s="1">
-        <v>950.4</v>
+        <v>982.8</v>
       </c>
       <c r="G15" s="1">
-        <v>948.1</v>
+        <v>980.9</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="15" x14ac:dyDescent="0.3">
@@ -868,22 +868,22 @@
         <v>15</v>
       </c>
       <c r="B16" s="1">
-        <v>950</v>
+        <v>973.9</v>
       </c>
       <c r="C16" s="1">
-        <v>948.4</v>
+        <v>979.6</v>
       </c>
       <c r="D16" s="1">
-        <v>948.8</v>
+        <v>979.8</v>
       </c>
       <c r="E16" s="1">
-        <v>949.4</v>
+        <v>979.3</v>
       </c>
       <c r="F16" s="1">
-        <v>951.2</v>
+        <v>981.6</v>
       </c>
       <c r="G16" s="1">
-        <v>948.9</v>
+        <v>977.6</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="15" x14ac:dyDescent="0.3">
@@ -891,22 +891,22 @@
         <v>16</v>
       </c>
       <c r="B17" s="1">
-        <v>949.5</v>
+        <v>972.6</v>
       </c>
       <c r="C17" s="1">
-        <v>950</v>
+        <v>976.4</v>
       </c>
       <c r="D17" s="1">
-        <v>948.7</v>
+        <v>977.5</v>
       </c>
       <c r="E17" s="1">
-        <v>951.6</v>
+        <v>977.1</v>
       </c>
       <c r="F17" s="1">
-        <v>948.7</v>
+        <v>977</v>
       </c>
       <c r="G17" s="1">
-        <v>947.3</v>
+        <v>975.7</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="15" x14ac:dyDescent="0.3">
@@ -914,22 +914,22 @@
         <v>17</v>
       </c>
       <c r="B18" s="1">
-        <v>949.4</v>
+        <v>973.7</v>
       </c>
       <c r="C18" s="1">
-        <v>947.6</v>
+        <v>974.8</v>
       </c>
       <c r="D18" s="1">
-        <v>947.1</v>
+        <v>979.3</v>
       </c>
       <c r="E18" s="1">
-        <v>948.5</v>
+        <v>978.3</v>
       </c>
       <c r="F18" s="1">
-        <v>951.4</v>
+        <v>981.1</v>
       </c>
       <c r="G18" s="1">
-        <v>948.5</v>
+        <v>978.4</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="15" x14ac:dyDescent="0.3">
@@ -937,22 +937,22 @@
         <v>18</v>
       </c>
       <c r="B19" s="1">
-        <v>949.1</v>
+        <v>970.6</v>
       </c>
       <c r="C19" s="1">
-        <v>949.5</v>
+        <v>979.6</v>
       </c>
       <c r="D19" s="1">
-        <v>948.6</v>
+        <v>976.1</v>
       </c>
       <c r="E19" s="1">
-        <v>950.9</v>
+        <v>976.5</v>
       </c>
       <c r="F19" s="1">
-        <v>949.5</v>
+        <v>980</v>
       </c>
       <c r="G19" s="1">
-        <v>948.6</v>
+        <v>977.8</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="15" x14ac:dyDescent="0.3">
@@ -960,22 +960,22 @@
         <v>19</v>
       </c>
       <c r="B20" s="1">
-        <v>949.6</v>
+        <v>975.6</v>
       </c>
       <c r="C20" s="1">
-        <v>948.9</v>
+        <v>976.3</v>
       </c>
       <c r="D20" s="1">
-        <v>949</v>
+        <v>977.4</v>
       </c>
       <c r="E20" s="1">
-        <v>949.8</v>
+        <v>976.4</v>
       </c>
       <c r="F20" s="1">
-        <v>949.8</v>
+        <v>980.3</v>
       </c>
       <c r="G20" s="1">
-        <v>948.5</v>
+        <v>975.4</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15" x14ac:dyDescent="0.3">
@@ -983,367 +983,22 @@
         <v>20</v>
       </c>
       <c r="B21" s="1">
-        <v>949.2</v>
+        <v>971.3</v>
       </c>
       <c r="C21" s="1">
-        <v>949.8</v>
+        <v>972.6</v>
       </c>
       <c r="D21" s="1">
-        <v>947.6</v>
+        <v>973.1</v>
       </c>
       <c r="E21" s="1">
-        <v>949.1</v>
+        <v>975.5</v>
       </c>
       <c r="F21" s="1">
-        <v>948.6</v>
+        <v>976</v>
       </c>
       <c r="G21" s="1">
-        <v>948.6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A22" s="7">
-        <v>21</v>
-      </c>
-      <c r="B22" s="1">
-        <v>950.1</v>
-      </c>
-      <c r="C22" s="1">
-        <v>951.1</v>
-      </c>
-      <c r="D22" s="1">
-        <v>949</v>
-      </c>
-      <c r="E22" s="1">
-        <v>951.1</v>
-      </c>
-      <c r="F22" s="1">
-        <v>949.1</v>
-      </c>
-      <c r="G22" s="1">
-        <v>950.7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A23" s="7">
-        <v>22</v>
-      </c>
-      <c r="B23" s="1">
-        <v>948.7</v>
-      </c>
-      <c r="C23" s="1">
-        <v>950</v>
-      </c>
-      <c r="D23" s="1">
-        <v>948.4</v>
-      </c>
-      <c r="E23" s="1">
-        <v>948.6</v>
-      </c>
-      <c r="F23" s="1">
-        <v>950.2</v>
-      </c>
-      <c r="G23" s="1">
-        <v>949.6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A24" s="7">
-        <v>23</v>
-      </c>
-      <c r="B24" s="1">
-        <v>949.5</v>
-      </c>
-      <c r="C24" s="1">
-        <v>949.3</v>
-      </c>
-      <c r="D24" s="1">
-        <v>948.6</v>
-      </c>
-      <c r="E24" s="1">
-        <v>947.6</v>
-      </c>
-      <c r="F24" s="1">
-        <v>949.5</v>
-      </c>
-      <c r="G24" s="1">
-        <v>950.5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A25" s="7">
-        <v>24</v>
-      </c>
-      <c r="B25" s="1">
-        <v>949.9</v>
-      </c>
-      <c r="C25" s="1">
-        <v>949.4</v>
-      </c>
-      <c r="D25" s="1">
-        <v>949.4</v>
-      </c>
-      <c r="E25" s="1">
-        <v>948.2</v>
-      </c>
-      <c r="F25" s="1">
-        <v>948.5</v>
-      </c>
-      <c r="G25" s="1">
-        <v>949.7</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A26" s="7">
-        <v>25</v>
-      </c>
-      <c r="B26" s="1">
-        <v>948.6</v>
-      </c>
-      <c r="C26" s="1">
-        <v>951.2</v>
-      </c>
-      <c r="D26" s="1">
-        <v>949.7</v>
-      </c>
-      <c r="E26" s="1">
-        <v>948</v>
-      </c>
-      <c r="F26" s="1">
-        <v>949.2</v>
-      </c>
-      <c r="G26" s="1">
-        <v>951</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A27" s="7">
-        <v>26</v>
-      </c>
-      <c r="B27" s="1">
-        <v>949.7</v>
-      </c>
-      <c r="C27" s="1">
-        <v>950.9</v>
-      </c>
-      <c r="D27" s="1">
-        <v>950.1</v>
-      </c>
-      <c r="E27" s="1">
-        <v>948.7</v>
-      </c>
-      <c r="F27" s="1">
-        <v>948.7</v>
-      </c>
-      <c r="G27" s="1">
-        <v>951</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A28" s="7">
-        <v>27</v>
-      </c>
-      <c r="B28" s="1">
-        <v>949.1</v>
-      </c>
-      <c r="C28" s="1">
-        <v>949.9</v>
-      </c>
-      <c r="D28" s="1">
-        <v>948.6</v>
-      </c>
-      <c r="E28" s="1">
-        <v>948.5</v>
-      </c>
-      <c r="F28" s="1">
-        <v>948.9</v>
-      </c>
-      <c r="G28" s="1">
-        <v>951.4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A29" s="7">
-        <v>28</v>
-      </c>
-      <c r="B29" s="1">
-        <v>949.3</v>
-      </c>
-      <c r="C29" s="1">
-        <v>950.6</v>
-      </c>
-      <c r="D29" s="1">
-        <v>949.6</v>
-      </c>
-      <c r="E29" s="1">
-        <v>948.6</v>
-      </c>
-      <c r="F29" s="1">
-        <v>950.2</v>
-      </c>
-      <c r="G29" s="1">
-        <v>947.5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A30" s="7">
-        <v>29</v>
-      </c>
-      <c r="B30" s="1">
-        <v>949.4</v>
-      </c>
-      <c r="C30" s="1">
-        <v>950.7</v>
-      </c>
-      <c r="D30" s="1">
-        <v>949.9</v>
-      </c>
-      <c r="E30" s="1">
-        <v>950.1</v>
-      </c>
-      <c r="F30" s="1">
-        <v>949.7</v>
-      </c>
-      <c r="G30" s="1">
-        <v>948.7</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A31" s="7">
-        <v>30</v>
-      </c>
-      <c r="B31" s="1">
-        <v>949</v>
-      </c>
-      <c r="C31" s="1">
-        <v>951.2</v>
-      </c>
-      <c r="D31" s="1">
-        <v>948.7</v>
-      </c>
-      <c r="E31" s="1">
-        <v>949.1</v>
-      </c>
-      <c r="F31" s="1">
-        <v>950.5</v>
-      </c>
-      <c r="G31" s="1">
-        <v>950.8</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A32" s="7">
-        <v>31</v>
-      </c>
-      <c r="B32" s="1">
-        <v>949.7</v>
-      </c>
-      <c r="C32" s="1">
-        <v>950.3</v>
-      </c>
-      <c r="D32" s="1">
-        <v>948.8</v>
-      </c>
-      <c r="E32" s="1">
-        <v>950.4</v>
-      </c>
-      <c r="F32" s="1">
-        <v>946.9</v>
-      </c>
-      <c r="G32" s="1">
-        <v>950.5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A33" s="7">
-        <v>32</v>
-      </c>
-      <c r="B33" s="1">
-        <v>949.4</v>
-      </c>
-      <c r="C33" s="1">
-        <v>951.2</v>
-      </c>
-      <c r="D33" s="1">
-        <v>950.5</v>
-      </c>
-      <c r="E33" s="1">
-        <v>948.8</v>
-      </c>
-      <c r="F33" s="1">
-        <v>949.5</v>
-      </c>
-      <c r="G33" s="1">
-        <v>951</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A34" s="7">
-        <v>33</v>
-      </c>
-      <c r="B34" s="1">
-        <v>949.6</v>
-      </c>
-      <c r="C34" s="1">
-        <v>951.6</v>
-      </c>
-      <c r="D34" s="1">
-        <v>949.6</v>
-      </c>
-      <c r="E34" s="1">
-        <v>949.6</v>
-      </c>
-      <c r="F34" s="1">
-        <v>950.6</v>
-      </c>
-      <c r="G34" s="1">
-        <v>949.4</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A35" s="7">
-        <v>34</v>
-      </c>
-      <c r="B35" s="1">
-        <v>949.6</v>
-      </c>
-      <c r="C35" s="1">
-        <v>950.5</v>
-      </c>
-      <c r="D35" s="1">
-        <v>949.5</v>
-      </c>
-      <c r="E35" s="1">
-        <v>949.8</v>
-      </c>
-      <c r="F35" s="1">
-        <v>950</v>
-      </c>
-      <c r="G35" s="1">
-        <v>951.9</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A36" s="7">
-        <v>35</v>
-      </c>
-      <c r="B36" s="1">
-        <v>949.6</v>
-      </c>
-      <c r="C36" s="1">
-        <v>950.5</v>
-      </c>
-      <c r="D36" s="1">
-        <v>950.2</v>
-      </c>
-      <c r="E36" s="1">
-        <v>949.3</v>
-      </c>
-      <c r="F36" s="1">
-        <v>949.8</v>
-      </c>
-      <c r="G36" s="1">
-        <v>950.3</v>
+        <v>976.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>